<commit_message>
modified Overlap degree is added
</commit_message>
<xml_diff>
--- a/Mapping/ToolsCapacity.xlsx
+++ b/Mapping/ToolsCapacity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shikahjs/Documents/MyFiles/PhDwork/MultiTagging/Mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D660055-17A2-DC4D-8FD5-A589D8281D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675E6962-0728-6C4B-B9BB-8B1581C02554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17180" xr2:uid="{63C0300A-8945-6C49-A339-1F2278BBE694}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{63C0300A-8945-6C49-A339-1F2278BBE694}"/>
   </bookViews>
   <sheets>
     <sheet name="DASP" sheetId="1" r:id="rId1"/>
@@ -171,9 +171,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -211,7 +211,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -317,7 +317,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -459,7 +459,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -469,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA5F0DFA-03B6-A145-8046-383B193B5719}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -550,7 +550,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -562,7 +562,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
@@ -591,7 +591,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
@@ -600,7 +600,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="4">
         <v>0</v>
@@ -626,7 +626,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Mythril has been upgraded to v.0.24.8.
</commit_message>
<xml_diff>
--- a/Mapping/ToolsCapacity.xlsx
+++ b/Mapping/ToolsCapacity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shikahjs/Documents/MyFiles/PhDwork/MultiTagging/Mapping/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shikahjs/Documents/MyFiles/PhDwork/MultiTagging [Edited] v2/Mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675E6962-0728-6C4B-B9BB-8B1581C02554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D29402-DDB0-0F42-8067-5F964A35C0DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{63C0300A-8945-6C49-A339-1F2278BBE694}"/>
+    <workbookView xWindow="15320" yWindow="740" windowWidth="14920" windowHeight="18900" xr2:uid="{63C0300A-8945-6C49-A339-1F2278BBE694}"/>
   </bookViews>
   <sheets>
     <sheet name="DASP" sheetId="1" r:id="rId1"/>
@@ -469,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA5F0DFA-03B6-A145-8046-383B193B5719}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -550,7 +550,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -562,13 +562,13 @@
         <v>1</v>
       </c>
       <c r="F3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
       </c>
       <c r="H3" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="1">
         <v>1</v>
@@ -591,7 +591,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
@@ -600,13 +600,13 @@
         <v>0</v>
       </c>
       <c r="G4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="4">
         <v>0</v>
       </c>
       <c r="I4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="4">
         <v>0</v>

</xml_diff>